<commit_message>
Changement excel liés au trigger + date jeux
</commit_message>
<xml_diff>
--- a/bdd_excel/Jeux.xlsx
+++ b/bdd_excel/Jeux.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/florianbour/Desktop/ENSEIRB/2A/SGBD/sgbd-jeux/bdd_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucap\Desktop\Ecole\ENSEIRB\S7\SGBD\Projet\bdd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8684D602-A853-6F46-81F7-D2E44E8BDB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595F7377-FCE8-4853-8429-D39A5B7C123F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15600" xr2:uid="{642E0B34-DEEB-4D43-8721-D90C3281AE4B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{642E0B34-DEEB-4D43-8721-D90C3281AE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -303,6 +303,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -332,8 +335,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FABA486F-CF32-0346-BC63-9A9464ABB015}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -698,8 +703,8 @@
       <c r="E2">
         <v>45</v>
       </c>
-      <c r="F2">
-        <v>2011</v>
+      <c r="F2" s="2">
+        <v>40544</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -707,8 +712,9 @@
       <c r="H2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -724,8 +730,8 @@
       <c r="E3">
         <v>30</v>
       </c>
-      <c r="F3">
-        <v>2019</v>
+      <c r="F3" s="2">
+        <v>43466</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -733,8 +739,9 @@
       <c r="H3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -750,8 +757,8 @@
       <c r="E4">
         <v>45</v>
       </c>
-      <c r="F4">
-        <v>2008</v>
+      <c r="F4" s="2">
+        <v>39448</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -759,8 +766,9 @@
       <c r="H4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -776,8 +784,8 @@
       <c r="E5">
         <v>40</v>
       </c>
-      <c r="F5">
-        <v>2015</v>
+      <c r="F5" s="2">
+        <v>42005</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -785,8 +793,9 @@
       <c r="H5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -802,8 +811,8 @@
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="F6">
-        <v>2018</v>
+      <c r="F6" s="2">
+        <v>43101</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -811,8 +820,9 @@
       <c r="H6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -828,8 +838,8 @@
       <c r="E7">
         <v>30</v>
       </c>
-      <c r="F7">
-        <v>2018</v>
+      <c r="F7" s="2">
+        <v>43101</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -837,8 +847,9 @@
       <c r="H7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -854,8 +865,8 @@
       <c r="E8">
         <v>45</v>
       </c>
-      <c r="F8">
-        <v>2014</v>
+      <c r="F8" s="2">
+        <v>41640</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -863,8 +874,9 @@
       <c r="H8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -880,8 +892,8 @@
       <c r="E9">
         <v>90</v>
       </c>
-      <c r="F9">
-        <v>2017</v>
+      <c r="F9" s="2">
+        <v>42736</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -889,8 +901,9 @@
       <c r="H9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -906,8 +919,8 @@
       <c r="E10">
         <v>80</v>
       </c>
-      <c r="F10">
-        <v>2017</v>
+      <c r="F10" s="2">
+        <v>42736</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -915,8 +928,9 @@
       <c r="H10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -932,8 +946,8 @@
       <c r="E11">
         <v>60</v>
       </c>
-      <c r="F11">
-        <v>2016</v>
+      <c r="F11" s="2">
+        <v>42370</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -941,8 +955,9 @@
       <c r="H11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -958,8 +973,8 @@
       <c r="E12">
         <v>60</v>
       </c>
-      <c r="F12">
-        <v>2014</v>
+      <c r="F12" s="2">
+        <v>41640</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -967,8 +982,9 @@
       <c r="H12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -984,8 +1000,8 @@
       <c r="E13">
         <v>60</v>
       </c>
-      <c r="F13">
-        <v>2017</v>
+      <c r="F13" s="2">
+        <v>42736</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -993,8 +1009,9 @@
       <c r="H13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1010,8 +1027,8 @@
       <c r="E14">
         <v>50</v>
       </c>
-      <c r="F14">
-        <v>2017</v>
+      <c r="F14" s="2">
+        <v>42736</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1019,8 +1036,9 @@
       <c r="H14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1036,8 +1054,8 @@
       <c r="E15">
         <v>45</v>
       </c>
-      <c r="F15">
-        <v>2018</v>
+      <c r="F15" s="2">
+        <v>43101</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -1045,8 +1063,9 @@
       <c r="H15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1062,8 +1081,8 @@
       <c r="E16">
         <v>90</v>
       </c>
-      <c r="F16">
-        <v>2012</v>
+      <c r="F16" s="2">
+        <v>40909</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -1071,8 +1090,9 @@
       <c r="H16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1088,8 +1108,8 @@
       <c r="E17">
         <v>30</v>
       </c>
-      <c r="F17">
-        <v>2010</v>
+      <c r="F17" s="2">
+        <v>40179</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -1097,8 +1117,9 @@
       <c r="H17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1114,8 +1135,8 @@
       <c r="E18">
         <v>60</v>
       </c>
-      <c r="F18">
-        <v>2017</v>
+      <c r="F18" s="2">
+        <v>42736</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -1123,8 +1144,9 @@
       <c r="H18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1140,8 +1162,8 @@
       <c r="E19">
         <v>45</v>
       </c>
-      <c r="F19">
-        <v>2017</v>
+      <c r="F19" s="2">
+        <v>42736</v>
       </c>
       <c r="G19">
         <v>2</v>
@@ -1149,8 +1171,9 @@
       <c r="H19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1166,8 +1189,8 @@
       <c r="E20">
         <v>45</v>
       </c>
-      <c r="F20">
-        <v>2018</v>
+      <c r="F20" s="2">
+        <v>43101</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1175,8 +1198,9 @@
       <c r="H20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1192,8 +1216,8 @@
       <c r="E21">
         <v>45</v>
       </c>
-      <c r="F21">
-        <v>2020</v>
+      <c r="F21" s="2">
+        <v>43831</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1201,8 +1225,9 @@
       <c r="H21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1218,8 +1243,8 @@
       <c r="E22">
         <v>25</v>
       </c>
-      <c r="F22">
-        <v>2021</v>
+      <c r="F22" s="2">
+        <v>44197</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -1227,8 +1252,9 @@
       <c r="H22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1244,8 +1270,8 @@
       <c r="E23">
         <v>45</v>
       </c>
-      <c r="F23">
-        <v>2017</v>
+      <c r="F23" s="2">
+        <v>42736</v>
       </c>
       <c r="G23">
         <v>2</v>
@@ -1253,8 +1279,9 @@
       <c r="H23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1270,8 +1297,8 @@
       <c r="E24">
         <v>60</v>
       </c>
-      <c r="F24">
-        <v>2019</v>
+      <c r="F24" s="2">
+        <v>43466</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1279,8 +1306,9 @@
       <c r="H24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1296,8 +1324,8 @@
       <c r="E25">
         <v>90</v>
       </c>
-      <c r="F25">
-        <v>2018</v>
+      <c r="F25" s="2">
+        <v>43101</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1305,8 +1333,9 @@
       <c r="H25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1322,8 +1351,8 @@
       <c r="E26">
         <v>45</v>
       </c>
-      <c r="F26">
-        <v>2009</v>
+      <c r="F26" s="2">
+        <v>39814</v>
       </c>
       <c r="G26">
         <v>3</v>
@@ -1331,8 +1360,9 @@
       <c r="H26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1348,8 +1378,8 @@
       <c r="E27">
         <v>45</v>
       </c>
-      <c r="F27">
-        <v>2019</v>
+      <c r="F27" s="2">
+        <v>43466</v>
       </c>
       <c r="G27">
         <v>2</v>
@@ -1357,8 +1387,9 @@
       <c r="H27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1374,8 +1405,8 @@
       <c r="E28">
         <v>75</v>
       </c>
-      <c r="F28">
-        <v>2007</v>
+      <c r="F28" s="2">
+        <v>39083</v>
       </c>
       <c r="G28">
         <v>3</v>
@@ -1383,8 +1414,9 @@
       <c r="H28">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1400,8 +1432,8 @@
       <c r="E29">
         <v>30</v>
       </c>
-      <c r="F29">
-        <v>2006</v>
+      <c r="F29" s="2">
+        <v>38718</v>
       </c>
       <c r="G29">
         <v>2</v>
@@ -1409,8 +1441,9 @@
       <c r="H29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1426,8 +1459,8 @@
       <c r="E30">
         <v>45</v>
       </c>
-      <c r="F30">
-        <v>2017</v>
+      <c r="F30" s="2">
+        <v>42736</v>
       </c>
       <c r="G30">
         <v>2</v>
@@ -1435,8 +1468,9 @@
       <c r="H30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1452,8 +1486,8 @@
       <c r="E31">
         <v>30</v>
       </c>
-      <c r="F31">
-        <v>2016</v>
+      <c r="F31" s="2">
+        <v>42370</v>
       </c>
       <c r="G31">
         <v>2</v>
@@ -1461,8 +1495,9 @@
       <c r="H31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1478,8 +1513,8 @@
       <c r="E32">
         <v>45</v>
       </c>
-      <c r="F32">
-        <v>2016</v>
+      <c r="F32" s="2">
+        <v>42370</v>
       </c>
       <c r="G32">
         <v>2</v>
@@ -1487,8 +1522,9 @@
       <c r="H32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1504,8 +1540,8 @@
       <c r="E33">
         <v>100</v>
       </c>
-      <c r="F33">
-        <v>2021</v>
+      <c r="F33" s="2">
+        <v>44197</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -1513,8 +1549,9 @@
       <c r="H33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1530,8 +1567,8 @@
       <c r="E34">
         <v>40</v>
       </c>
-      <c r="F34">
-        <v>2014</v>
+      <c r="F34" s="2">
+        <v>41640</v>
       </c>
       <c r="G34">
         <v>4</v>
@@ -1539,8 +1576,9 @@
       <c r="H34">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1556,8 +1594,8 @@
       <c r="E35">
         <v>30</v>
       </c>
-      <c r="F35">
-        <v>2014</v>
+      <c r="F35" s="2">
+        <v>41640</v>
       </c>
       <c r="G35">
         <v>3</v>
@@ -1565,8 +1603,9 @@
       <c r="H35">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1582,8 +1621,8 @@
       <c r="E36">
         <v>30</v>
       </c>
-      <c r="F36">
-        <v>2018</v>
+      <c r="F36" s="2">
+        <v>43101</v>
       </c>
       <c r="G36">
         <v>2</v>
@@ -1591,8 +1630,9 @@
       <c r="H36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1608,8 +1648,8 @@
       <c r="E37">
         <v>100</v>
       </c>
-      <c r="F37">
-        <v>2016</v>
+      <c r="F37" s="2">
+        <v>42370</v>
       </c>
       <c r="G37">
         <v>2</v>
@@ -1617,8 +1657,9 @@
       <c r="H37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1634,8 +1675,8 @@
       <c r="E38">
         <v>60</v>
       </c>
-      <c r="F38">
-        <v>2014</v>
+      <c r="F38" s="2">
+        <v>41640</v>
       </c>
       <c r="G38">
         <v>2</v>
@@ -1643,8 +1684,9 @@
       <c r="H38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1660,8 +1702,8 @@
       <c r="E39">
         <v>40</v>
       </c>
-      <c r="F39">
-        <v>2019</v>
+      <c r="F39" s="2">
+        <v>43466</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1669,8 +1711,9 @@
       <c r="H39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1686,8 +1729,8 @@
       <c r="E40">
         <v>30</v>
       </c>
-      <c r="F40">
-        <v>2017</v>
+      <c r="F40" s="2">
+        <v>42736</v>
       </c>
       <c r="G40">
         <v>2</v>
@@ -1695,8 +1738,9 @@
       <c r="H40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1712,8 +1756,8 @@
       <c r="E41">
         <v>45</v>
       </c>
-      <c r="F41">
-        <v>2014</v>
+      <c r="F41" s="2">
+        <v>41640</v>
       </c>
       <c r="G41">
         <v>2</v>
@@ -1721,8 +1765,9 @@
       <c r="H41">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1738,8 +1783,8 @@
       <c r="E42">
         <v>15</v>
       </c>
-      <c r="F42">
-        <v>2016</v>
+      <c r="F42" s="2">
+        <v>42370</v>
       </c>
       <c r="G42">
         <v>2</v>
@@ -1747,8 +1792,9 @@
       <c r="H42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1764,8 +1810,8 @@
       <c r="E43">
         <v>15</v>
       </c>
-      <c r="F43">
-        <v>2016</v>
+      <c r="F43" s="2">
+        <v>42370</v>
       </c>
       <c r="G43">
         <v>2</v>
@@ -1773,8 +1819,9 @@
       <c r="H43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1790,8 +1837,8 @@
       <c r="E44">
         <v>25</v>
       </c>
-      <c r="F44">
-        <v>2017</v>
+      <c r="F44" s="2">
+        <v>42736</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -1799,8 +1846,9 @@
       <c r="H44">
         <v>100</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1816,8 +1864,8 @@
       <c r="E45">
         <v>25</v>
       </c>
-      <c r="F45">
-        <v>2019</v>
+      <c r="F45" s="2">
+        <v>43466</v>
       </c>
       <c r="G45">
         <v>2</v>
@@ -1825,8 +1873,9 @@
       <c r="H45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1842,8 +1891,8 @@
       <c r="E46">
         <v>30</v>
       </c>
-      <c r="F46">
-        <v>2015</v>
+      <c r="F46" s="2">
+        <v>42005</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -1851,8 +1900,9 @@
       <c r="H46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1868,8 +1918,8 @@
       <c r="E47">
         <v>30</v>
       </c>
-      <c r="F47">
-        <v>2020</v>
+      <c r="F47" s="2">
+        <v>43831</v>
       </c>
       <c r="G47">
         <v>2</v>
@@ -1877,8 +1927,9 @@
       <c r="H47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1894,8 +1945,8 @@
       <c r="E48">
         <v>30</v>
       </c>
-      <c r="F48">
-        <v>2019</v>
+      <c r="F48" s="2">
+        <v>43466</v>
       </c>
       <c r="G48">
         <v>2</v>
@@ -1903,8 +1954,9 @@
       <c r="H48">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1920,8 +1972,8 @@
       <c r="E49">
         <v>40</v>
       </c>
-      <c r="F49">
-        <v>2015</v>
+      <c r="F49" s="2">
+        <v>42005</v>
       </c>
       <c r="G49">
         <v>2</v>
@@ -1929,8 +1981,9 @@
       <c r="H49">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1946,8 +1999,8 @@
       <c r="E50">
         <v>30</v>
       </c>
-      <c r="F50">
-        <v>2017</v>
+      <c r="F50" s="2">
+        <v>42736</v>
       </c>
       <c r="G50">
         <v>2</v>
@@ -1955,8 +2008,9 @@
       <c r="H50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1972,8 +2026,8 @@
       <c r="E51">
         <v>30</v>
       </c>
-      <c r="F51">
-        <v>2014</v>
+      <c r="F51" s="2">
+        <v>41640</v>
       </c>
       <c r="G51">
         <v>2</v>
@@ -1981,8 +2035,10 @@
       <c r="H51">
         <v>4</v>
       </c>
+      <c r="J51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nouvelle essai format Date Jeux
</commit_message>
<xml_diff>
--- a/bdd_excel/Jeux.xlsx
+++ b/bdd_excel/Jeux.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucap\Desktop\Ecole\ENSEIRB\S7\SGBD\Projet\bdd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673033F8-FDC1-4B61-A653-A6DB4A3DEDF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E16E9D-5C03-45EC-B2EA-1CBC5F7D8477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{642E0B34-DEEB-4D43-8721-D90C3281AE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -304,7 +304,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="\'yyyy\'"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -655,7 +655,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Nouvelle essai V2 format Date Jeux
</commit_message>
<xml_diff>
--- a/bdd_excel/Jeux.xlsx
+++ b/bdd_excel/Jeux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucap\Desktop\Ecole\ENSEIRB\S7\SGBD\Projet\bdd_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E16E9D-5C03-45EC-B2EA-1CBC5F7D8477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C2561-1500-48B1-9D5E-ABCC8DACD992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{642E0B34-DEEB-4D43-8721-D90C3281AE4B}"/>
   </bookViews>
@@ -304,7 +304,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="\'yyyy\'"/>
+    <numFmt numFmtId="165" formatCode="\'yyyy\-mm\-dd\'"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -337,7 +337,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +655,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>